<commit_message>
Push existing project to ExpenseTrackerMobileApp repo
</commit_message>
<xml_diff>
--- a/assets/Expense_Template.xlsx
+++ b/assets/Expense_Template.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28526"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B2FF8CC-A25C-438A-87EB-F1DC79065A0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{542EFED2-0CC4-43C5-8E45-7717FA0FDB19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21697" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
   <si>
     <t xml:space="preserve">EXPENSES &amp; TRAVEL REIMBURSEMENT FORM </t>
   </si>
@@ -110,25 +110,13 @@
     <t>{{Today's Date}}</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t xml:space="preserve"> Date：</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <u/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-      </rPr>
-      <t xml:space="preserve">          _{{Today's Date}}____________</t>
-    </r>
+    <t>Date:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          _{{Today's Date}}____________</t>
+  </si>
+  <si>
+    <t>___{{Full Name}}_______</t>
   </si>
 </sst>
 </file>
@@ -140,7 +128,7 @@
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0;[Red]\-&quot;$&quot;#,##0"/>
     <numFmt numFmtId="165" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="15">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -233,12 +221,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <b/>
       <u/>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -389,7 +371,7 @@
     </xf>
     <xf numFmtId="43" fontId="12" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -505,7 +487,7 @@
     <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -546,6 +528,9 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="8" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -911,8 +896,8 @@
   </sheetPr>
   <dimension ref="A3:F63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView tabSelected="1" topLeftCell="A50" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C61" sqref="C61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="13.5"/>
@@ -1340,7 +1325,7 @@
         <v>11</v>
       </c>
       <c r="B57" s="38" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C57" s="24"/>
       <c r="D57" s="24"/>
@@ -1352,9 +1337,11 @@
       </c>
       <c r="B58" s="39"/>
       <c r="C58" s="11"/>
-      <c r="D58" s="11"/>
+      <c r="D58" s="55" t="s">
+        <v>18</v>
+      </c>
       <c r="E58" s="41" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="59" spans="1:5" s="7" customFormat="1" ht="34.35" customHeight="1">

</xml_diff>